<commit_message>
Melhorias na estrutura de arquivos.
</commit_message>
<xml_diff>
--- a/FluentQnA/ConsoleApplication/knowledgebase.xlsx
+++ b/FluentQnA/ConsoleApplication/knowledgebase.xlsx
@@ -1,72 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo Júnior\source\repos\FluentQnA\FluentQnA\WebApplication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\source\repos\snowflakesss\FluentQnA\FluentQnA\ConsoleApplication\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52DFE08-B51F-4274-9B29-C847EDBAF45A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18600" windowHeight="7140"/>
+    <workbookView xWindow="90" yWindow="210" windowWidth="17910" windowHeight="10410" xr2:uid="{21AE095E-EF90-4A1C-A6B1-AF72FB63EAF8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Qual seu nome?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    Questions</t>
-  </si>
-  <si>
-    <t>Você tem nome ?</t>
-  </si>
-  <si>
-    <t>FluentQnA</t>
-  </si>
-  <si>
-    <t>Sou um serviço cognitivo para responder perguntas de usuários consultando uma base de conhecimento.</t>
-  </si>
-  <si>
-    <t>O que você faz ?</t>
-  </si>
-  <si>
-    <t>Para o que você server?</t>
-  </si>
-  <si>
-    <t>Quem é você?</t>
-  </si>
-  <si>
-    <t>Como posso te utilizar?</t>
-  </si>
-  <si>
-    <t>Posso ser utilizado para chatbots ou serviços de suporte e perguntas frequentes.</t>
-  </si>
-  <si>
-    <t>qual sua aplicabilidade ?</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>qual o seu nome?</t>
+  </si>
+  <si>
+    <t>você tem algum nome ?</t>
+  </si>
+  <si>
+    <t>meu nome é FluentQnA</t>
+  </si>
+  <si>
+    <t>o que você pode fazer ?</t>
+  </si>
+  <si>
+    <t>eu posso usar aprendizado de máquina para tentar responder perguntas de usuários consultando uma base de conhecimento</t>
+  </si>
+  <si>
+    <t>o que exatamente você faz ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,22 +69,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -97,60 +94,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -171,7 +122,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +136,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -197,7 +148,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -209,14 +160,14 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -244,14 +195,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -279,9 +247,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -430,93 +415,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B566A58E-DA4C-4F4A-8C65-8A22D8E1C427}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:Z1"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>